<commit_message>
corrección graficas y preguntas
falata corregir las descripciones
</commit_message>
<xml_diff>
--- a/.estadisticaentorno/uploads/Cuentas_con_redes.xlsx
+++ b/.estadisticaentorno/uploads/Cuentas_con_redes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\5TO SEMESTRE\ESTADISTICA II\proyectoestadistica2.0\.estadisticaentorno\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818A7DDE-8A70-4038-A6F9-1540ED66CAAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B46A47-6D3E-4597-BB3F-EC179C66D3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -366,10 +366,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>